<commit_message>
readme update + шефы
</commit_message>
<xml_diff>
--- a/шефы.xlsx
+++ b/шефы.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2508" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="3108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Шефы</t>
   </si>
@@ -77,24 +77,6 @@
   </si>
   <si>
     <t>Шоть Ксения Сергеевна</t>
-  </si>
-  <si>
-    <t>Иванов Андрей Александрович</t>
-  </si>
-  <si>
-    <t>Курилович Даниил Геннадьевич</t>
-  </si>
-  <si>
-    <t>Раджабов Осаф Манучехрович</t>
-  </si>
-  <si>
-    <t>Скоков Андрей Владимирович</t>
-  </si>
-  <si>
-    <t>Урбанович Антон Александрович</t>
-  </si>
-  <si>
-    <t>Шмаргун Александр Эдуардович</t>
   </si>
   <si>
     <t>Карась Андрей Сергеевич(3)</t>
@@ -554,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -582,7 +564,7 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -623,142 +605,123 @@
     </row>
     <row r="9" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6"/>
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>32</v>
+      <c r="A12" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>31</v>
+      <c r="A14" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>11</v>
+      <c r="A15" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
-        <v>29</v>
+    <row r="25" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>18</v>
-      </c>
+    <row r="26" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>25</v>
-      </c>
+    <row r="27" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>30</v>
-      </c>
+    <row r="28" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>19</v>
-      </c>
+    <row r="29" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>26</v>
-      </c>
+    <row r="30" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6"/>
     </row>
     <row r="31" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="B31" s="6"/>
     </row>
   </sheetData>

</xml_diff>